<commit_message>
Updated assessment areas to v8b. Renamed Coastal DEDK Outer Coastal DEDK (OC) as agreed at ICG-EUT.
</commit_message>
<xml_diff>
--- a/assessment_areas/Assessment_area_definition.xlsx
+++ b/assessment_areas/Assessment_area_definition.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cefas-my.sharepoint.com/personal/kate_collingridge_cefas_co_uk/Documents/COMPEAT/assessment_areas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FA6F7655-D343-4A2C-81B0-6C1A9E7C1512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="8_{FA6F7655-D343-4A2C-81B0-6C1A9E7C1512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{65B9C7BA-266B-4C77-94D0-2005384B39D6}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6FFA0BA9-2905-471C-BEB8-3064AD9CC18F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{6FFA0BA9-2905-471C-BEB8-3064AD9CC18F}"/>
   </bookViews>
   <sheets>
     <sheet name="Descriptions" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="347">
   <si>
     <t>Version of shapefile</t>
   </si>
@@ -1071,10 +1071,16 @@
     <t>Updated Portuguese areas. They essentially combine intermediate and coastal waters. Realigned with EEZ and removed a couple of fragment polygons. Renamed Coastal Offshore to Coastal DEDK as agreed at TG-COMP 5.</t>
   </si>
   <si>
-    <t>CODEDK</t>
-  </si>
-  <si>
-    <t>Coastal DEDK</t>
+    <t>OC</t>
+  </si>
+  <si>
+    <t>Outer Coastal DEDK</t>
+  </si>
+  <si>
+    <t>COMP4_assessment_areas_v8b</t>
+  </si>
+  <si>
+    <t>Minor edits to remove overlaps. Renamed Coastal DEDK Outer Coastal DEDK (OC) as agreed at ICG-EUT.</t>
   </si>
 </sst>
 </file>
@@ -1282,28 +1288,11 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1311,6 +1300,23 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1627,11 +1633,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F019ECE8-FE8C-43D4-8973-CA53C99D866F}">
   <dimension ref="A1:S110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D24" sqref="D24:D25"/>
+      <selection pane="bottomRight" activeCell="C24" sqref="C24:C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1801,22 +1807,22 @@
       </c>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="41" t="s">
+      <c r="C4" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="42" t="s">
+      <c r="D4" s="50" t="s">
         <v>139</v>
       </c>
-      <c r="E4" s="43" t="s">
+      <c r="E4" s="47" t="s">
         <v>140</v>
       </c>
-      <c r="F4" s="44" t="s">
+      <c r="F4" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="43" t="s">
+      <c r="G4" s="47" t="s">
         <v>14</v>
       </c>
       <c r="H4" s="6" t="s">
@@ -1830,13 +1836,13 @@
       <c r="L4" s="39">
         <v>217300.885052</v>
       </c>
-      <c r="M4" s="40">
+      <c r="M4" s="41">
         <v>35.160357250734101</v>
       </c>
-      <c r="N4" s="40">
+      <c r="N4" s="41">
         <v>34.690494537353501</v>
       </c>
-      <c r="O4" s="40">
+      <c r="O4" s="41">
         <v>35.458530426025398</v>
       </c>
       <c r="P4" s="39">
@@ -1850,12 +1856,12 @@
       </c>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B5" s="41"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="43"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="47"/>
       <c r="H5" s="6" t="s">
         <v>19</v>
       </c>
@@ -1865,20 +1871,20 @@
       <c r="J5" s="6"/>
       <c r="K5" s="6"/>
       <c r="L5" s="39"/>
-      <c r="M5" s="40"/>
-      <c r="N5" s="40"/>
-      <c r="O5" s="40"/>
+      <c r="M5" s="41"/>
+      <c r="N5" s="41"/>
+      <c r="O5" s="41"/>
       <c r="P5" s="39"/>
       <c r="Q5" s="39"/>
       <c r="R5" s="39"/>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B6" s="41"/>
-      <c r="C6" s="41"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="43"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="47"/>
       <c r="H6" s="6" t="s">
         <v>92</v>
       </c>
@@ -1888,20 +1894,20 @@
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
       <c r="L6" s="39"/>
-      <c r="M6" s="40"/>
-      <c r="N6" s="40"/>
-      <c r="O6" s="40"/>
+      <c r="M6" s="41"/>
+      <c r="N6" s="41"/>
+      <c r="O6" s="41"/>
       <c r="P6" s="39"/>
       <c r="Q6" s="39"/>
       <c r="R6" s="39"/>
     </row>
     <row r="7" spans="2:18" ht="45" x14ac:dyDescent="0.25">
-      <c r="B7" s="41"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="44"/>
-      <c r="F7" s="44"/>
-      <c r="G7" s="43"/>
+      <c r="B7" s="46"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="48"/>
+      <c r="F7" s="48"/>
+      <c r="G7" s="47"/>
       <c r="H7" s="6" t="s">
         <v>21</v>
       </c>
@@ -1911,30 +1917,30 @@
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
       <c r="L7" s="39"/>
-      <c r="M7" s="40"/>
-      <c r="N7" s="40"/>
-      <c r="O7" s="40"/>
+      <c r="M7" s="41"/>
+      <c r="N7" s="41"/>
+      <c r="O7" s="41"/>
       <c r="P7" s="39"/>
       <c r="Q7" s="39"/>
       <c r="R7" s="39"/>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B8" s="41" t="s">
+      <c r="B8" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="41" t="s">
+      <c r="C8" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="42" t="s">
+      <c r="D8" s="50" t="s">
         <v>141</v>
       </c>
-      <c r="E8" s="43" t="s">
+      <c r="E8" s="47" t="s">
         <v>142</v>
       </c>
-      <c r="F8" s="44" t="s">
+      <c r="F8" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="43" t="s">
+      <c r="G8" s="47" t="s">
         <v>26</v>
       </c>
       <c r="H8" s="6" t="s">
@@ -1950,13 +1956,13 @@
       <c r="L8" s="39">
         <v>5081.0040239999998</v>
       </c>
-      <c r="M8" s="40">
+      <c r="M8" s="41">
         <v>34.839983599411902</v>
       </c>
-      <c r="N8" s="40">
+      <c r="N8" s="41">
         <v>34.700817108154297</v>
       </c>
-      <c r="O8" s="40">
+      <c r="O8" s="41">
         <v>34.968365478515601</v>
       </c>
       <c r="P8" s="39">
@@ -1970,12 +1976,12 @@
       </c>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B9" s="41"/>
-      <c r="C9" s="41"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="44"/>
-      <c r="F9" s="44"/>
-      <c r="G9" s="43"/>
+      <c r="B9" s="46"/>
+      <c r="C9" s="46"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="47"/>
       <c r="H9" s="6" t="s">
         <v>28</v>
       </c>
@@ -1985,30 +1991,30 @@
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
       <c r="L9" s="39"/>
-      <c r="M9" s="40"/>
-      <c r="N9" s="40"/>
-      <c r="O9" s="40"/>
+      <c r="M9" s="41"/>
+      <c r="N9" s="41"/>
+      <c r="O9" s="41"/>
       <c r="P9" s="39"/>
       <c r="Q9" s="39"/>
       <c r="R9" s="39"/>
     </row>
     <row r="10" spans="2:18" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="41" t="s">
+      <c r="C10" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="42" t="s">
+      <c r="D10" s="50" t="s">
         <v>141</v>
       </c>
-      <c r="E10" s="43" t="s">
+      <c r="E10" s="47" t="s">
         <v>144</v>
       </c>
-      <c r="F10" s="44" t="s">
+      <c r="F10" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="G10" s="43" t="s">
+      <c r="G10" s="47" t="s">
         <v>265</v>
       </c>
       <c r="H10" s="6" t="s">
@@ -2022,13 +2028,13 @@
       <c r="L10" s="39">
         <v>42015.312512999997</v>
       </c>
-      <c r="M10" s="40">
+      <c r="M10" s="41">
         <v>35.133432242293601</v>
       </c>
-      <c r="N10" s="40">
+      <c r="N10" s="41">
         <v>34.979557037353501</v>
       </c>
-      <c r="O10" s="40">
+      <c r="O10" s="41">
         <v>35.244640350341797</v>
       </c>
       <c r="P10" s="39">
@@ -2042,12 +2048,12 @@
       </c>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B11" s="41"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="44"/>
-      <c r="G11" s="43"/>
+      <c r="B11" s="46"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="48"/>
+      <c r="G11" s="47"/>
       <c r="H11" s="6" t="s">
         <v>27</v>
       </c>
@@ -2059,20 +2065,20 @@
         <v>180</v>
       </c>
       <c r="L11" s="39"/>
-      <c r="M11" s="40"/>
-      <c r="N11" s="40"/>
-      <c r="O11" s="40"/>
+      <c r="M11" s="41"/>
+      <c r="N11" s="41"/>
+      <c r="O11" s="41"/>
       <c r="P11" s="39"/>
       <c r="Q11" s="39"/>
       <c r="R11" s="39"/>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B12" s="41"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="42"/>
-      <c r="E12" s="43"/>
-      <c r="F12" s="44"/>
-      <c r="G12" s="43"/>
+      <c r="B12" s="46"/>
+      <c r="C12" s="46"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="47"/>
       <c r="H12" s="6" t="s">
         <v>34</v>
       </c>
@@ -2084,30 +2090,30 @@
       </c>
       <c r="K12" s="6"/>
       <c r="L12" s="39"/>
-      <c r="M12" s="40"/>
-      <c r="N12" s="40"/>
-      <c r="O12" s="40"/>
+      <c r="M12" s="41"/>
+      <c r="N12" s="41"/>
+      <c r="O12" s="41"/>
       <c r="P12" s="39"/>
       <c r="Q12" s="39"/>
       <c r="R12" s="39"/>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B13" s="41" t="s">
+      <c r="B13" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="41" t="s">
+      <c r="C13" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="42" t="s">
+      <c r="D13" s="50" t="s">
         <v>141</v>
       </c>
-      <c r="E13" s="42" t="s">
+      <c r="E13" s="50" t="s">
         <v>145</v>
       </c>
-      <c r="F13" s="44" t="s">
+      <c r="F13" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="G13" s="43" t="s">
+      <c r="G13" s="47" t="s">
         <v>38</v>
       </c>
       <c r="H13" s="6" t="s">
@@ -2123,13 +2129,13 @@
       <c r="L13" s="39">
         <v>20631.964479999999</v>
       </c>
-      <c r="M13" s="40">
+      <c r="M13" s="41">
         <v>35.001150390373297</v>
       </c>
-      <c r="N13" s="40">
+      <c r="N13" s="41">
         <v>34.828578948974602</v>
       </c>
-      <c r="O13" s="40">
+      <c r="O13" s="41">
         <v>35.130928039550803</v>
       </c>
       <c r="P13" s="39">
@@ -2143,12 +2149,12 @@
       </c>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B14" s="41"/>
-      <c r="C14" s="41"/>
-      <c r="D14" s="42"/>
-      <c r="E14" s="42"/>
-      <c r="F14" s="44"/>
-      <c r="G14" s="43"/>
+      <c r="B14" s="46"/>
+      <c r="C14" s="46"/>
+      <c r="D14" s="50"/>
+      <c r="E14" s="50"/>
+      <c r="F14" s="48"/>
+      <c r="G14" s="47"/>
       <c r="H14" s="6" t="s">
         <v>23</v>
       </c>
@@ -2160,20 +2166,20 @@
         <v>180</v>
       </c>
       <c r="L14" s="39"/>
-      <c r="M14" s="40"/>
-      <c r="N14" s="40"/>
-      <c r="O14" s="40"/>
+      <c r="M14" s="41"/>
+      <c r="N14" s="41"/>
+      <c r="O14" s="41"/>
       <c r="P14" s="39"/>
       <c r="Q14" s="39"/>
       <c r="R14" s="39"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B15" s="41"/>
-      <c r="C15" s="41"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="44"/>
-      <c r="G15" s="43"/>
+      <c r="B15" s="46"/>
+      <c r="C15" s="46"/>
+      <c r="D15" s="50"/>
+      <c r="E15" s="50"/>
+      <c r="F15" s="48"/>
+      <c r="G15" s="47"/>
       <c r="H15" s="6" t="s">
         <v>34</v>
       </c>
@@ -2185,20 +2191,20 @@
       </c>
       <c r="K15" s="6"/>
       <c r="L15" s="39"/>
-      <c r="M15" s="40"/>
-      <c r="N15" s="40"/>
-      <c r="O15" s="40"/>
+      <c r="M15" s="41"/>
+      <c r="N15" s="41"/>
+      <c r="O15" s="41"/>
       <c r="P15" s="39"/>
       <c r="Q15" s="39"/>
       <c r="R15" s="39"/>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B16" s="41"/>
-      <c r="C16" s="41"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="42"/>
-      <c r="F16" s="44"/>
-      <c r="G16" s="43"/>
+      <c r="B16" s="46"/>
+      <c r="C16" s="46"/>
+      <c r="D16" s="50"/>
+      <c r="E16" s="50"/>
+      <c r="F16" s="48"/>
+      <c r="G16" s="47"/>
       <c r="H16" s="6" t="s">
         <v>39</v>
       </c>
@@ -2210,30 +2216,30 @@
         <v>180</v>
       </c>
       <c r="L16" s="39"/>
-      <c r="M16" s="40"/>
-      <c r="N16" s="40"/>
-      <c r="O16" s="40"/>
+      <c r="M16" s="41"/>
+      <c r="N16" s="41"/>
+      <c r="O16" s="41"/>
       <c r="P16" s="39"/>
       <c r="Q16" s="39"/>
       <c r="R16" s="39"/>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B17" s="41" t="s">
+      <c r="B17" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="41" t="s">
+      <c r="C17" s="46" t="s">
         <v>40</v>
       </c>
-      <c r="D17" s="42" t="s">
+      <c r="D17" s="50" t="s">
         <v>141</v>
       </c>
-      <c r="E17" s="42" t="s">
+      <c r="E17" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="F17" s="44" t="s">
+      <c r="F17" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="G17" s="43"/>
+      <c r="G17" s="47"/>
       <c r="H17" s="6" t="s">
         <v>27</v>
       </c>
@@ -2247,13 +2253,13 @@
       <c r="L17" s="39">
         <v>7176.2928410000004</v>
       </c>
-      <c r="M17" s="40">
+      <c r="M17" s="41">
         <v>34.160878249531301</v>
       </c>
-      <c r="N17" s="40">
+      <c r="N17" s="41">
         <v>33.499618530273402</v>
       </c>
-      <c r="O17" s="40">
+      <c r="O17" s="41">
         <v>34.711925506591797</v>
       </c>
       <c r="P17" s="39">
@@ -2267,12 +2273,12 @@
       </c>
     </row>
     <row r="18" spans="2:18" ht="87.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="41"/>
-      <c r="C18" s="41"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42"/>
-      <c r="F18" s="44"/>
-      <c r="G18" s="43"/>
+      <c r="B18" s="46"/>
+      <c r="C18" s="46"/>
+      <c r="D18" s="50"/>
+      <c r="E18" s="50"/>
+      <c r="F18" s="48"/>
+      <c r="G18" s="47"/>
       <c r="H18" s="6" t="s">
         <v>42</v>
       </c>
@@ -2284,30 +2290,30 @@
         <v>180</v>
       </c>
       <c r="L18" s="39"/>
-      <c r="M18" s="40"/>
-      <c r="N18" s="40"/>
-      <c r="O18" s="40"/>
+      <c r="M18" s="41"/>
+      <c r="N18" s="41"/>
+      <c r="O18" s="41"/>
       <c r="P18" s="39"/>
       <c r="Q18" s="39"/>
       <c r="R18" s="39"/>
     </row>
     <row r="19" spans="2:18" ht="45" x14ac:dyDescent="0.25">
-      <c r="B19" s="41" t="s">
+      <c r="B19" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="41" t="s">
+      <c r="C19" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="D19" s="42" t="s">
+      <c r="D19" s="50" t="s">
         <v>147</v>
       </c>
-      <c r="E19" s="43" t="s">
+      <c r="E19" s="47" t="s">
         <v>148</v>
       </c>
-      <c r="F19" s="44" t="s">
+      <c r="F19" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="G19" s="43" t="s">
+      <c r="G19" s="47" t="s">
         <v>44</v>
       </c>
       <c r="H19" s="6" t="s">
@@ -2321,13 +2327,13 @@
       <c r="L19" s="39">
         <v>9583.2755899999993</v>
       </c>
-      <c r="M19" s="40">
+      <c r="M19" s="41">
         <v>33.9903422071663</v>
       </c>
-      <c r="N19" s="40">
+      <c r="N19" s="41">
         <v>33.740700912475603</v>
       </c>
-      <c r="O19" s="40">
+      <c r="O19" s="41">
         <v>34.286895751953097</v>
       </c>
       <c r="P19" s="39">
@@ -2341,12 +2347,12 @@
       </c>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B20" s="41"/>
-      <c r="C20" s="41"/>
-      <c r="D20" s="42"/>
-      <c r="E20" s="43"/>
-      <c r="F20" s="44"/>
-      <c r="G20" s="43"/>
+      <c r="B20" s="46"/>
+      <c r="C20" s="46"/>
+      <c r="D20" s="50"/>
+      <c r="E20" s="47"/>
+      <c r="F20" s="48"/>
+      <c r="G20" s="47"/>
       <c r="H20" s="6" t="s">
         <v>92</v>
       </c>
@@ -2356,9 +2362,9 @@
       <c r="J20" s="6"/>
       <c r="K20" s="6"/>
       <c r="L20" s="39"/>
-      <c r="M20" s="40"/>
-      <c r="N20" s="40"/>
-      <c r="O20" s="40"/>
+      <c r="M20" s="41"/>
+      <c r="N20" s="41"/>
+      <c r="O20" s="41"/>
       <c r="P20" s="39"/>
       <c r="Q20" s="39"/>
       <c r="R20" s="39"/>
@@ -2505,22 +2511,22 @@
       </c>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B24" s="41" t="s">
+      <c r="B24" s="46" t="s">
         <v>343</v>
       </c>
-      <c r="C24" s="41" t="s">
+      <c r="C24" s="46" t="s">
         <v>344</v>
       </c>
-      <c r="D24" s="42" t="s">
+      <c r="D24" s="50" t="s">
         <v>149</v>
       </c>
-      <c r="E24" s="42" t="s">
+      <c r="E24" s="50" t="s">
         <v>249</v>
       </c>
-      <c r="F24" s="44" t="s">
+      <c r="F24" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="G24" s="43"/>
+      <c r="G24" s="47"/>
       <c r="H24" s="18" t="s">
         <v>67</v>
       </c>
@@ -2532,13 +2538,13 @@
       <c r="L24" s="39">
         <v>18540.398615999999</v>
       </c>
-      <c r="M24" s="40">
+      <c r="M24" s="41">
         <v>33.363634972636497</v>
       </c>
-      <c r="N24" s="40">
+      <c r="N24" s="41">
         <v>32.519149780273402</v>
       </c>
-      <c r="O24" s="40">
+      <c r="O24" s="41">
         <v>34.097171783447301</v>
       </c>
       <c r="P24" s="39">
@@ -2552,12 +2558,12 @@
       </c>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B25" s="41"/>
-      <c r="C25" s="41"/>
-      <c r="D25" s="42"/>
-      <c r="E25" s="42"/>
-      <c r="F25" s="44"/>
-      <c r="G25" s="43"/>
+      <c r="B25" s="46"/>
+      <c r="C25" s="46"/>
+      <c r="D25" s="50"/>
+      <c r="E25" s="50"/>
+      <c r="F25" s="48"/>
+      <c r="G25" s="47"/>
       <c r="H25" s="18" t="s">
         <v>65</v>
       </c>
@@ -2569,9 +2575,9 @@
       </c>
       <c r="K25" s="6"/>
       <c r="L25" s="39"/>
-      <c r="M25" s="40"/>
-      <c r="N25" s="40"/>
-      <c r="O25" s="40"/>
+      <c r="M25" s="41"/>
+      <c r="N25" s="41"/>
+      <c r="O25" s="41"/>
       <c r="P25" s="39"/>
       <c r="Q25" s="39"/>
       <c r="R25" s="39"/>
@@ -2820,22 +2826,22 @@
       </c>
     </row>
     <row r="31" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="41" t="s">
+      <c r="B31" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="C31" s="41" t="s">
+      <c r="C31" s="46" t="s">
         <v>66</v>
       </c>
-      <c r="D31" s="42" t="s">
+      <c r="D31" s="50" t="s">
         <v>154</v>
       </c>
-      <c r="E31" s="43" t="s">
+      <c r="E31" s="47" t="s">
         <v>251</v>
       </c>
-      <c r="F31" s="44" t="s">
+      <c r="F31" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="G31" s="43"/>
+      <c r="G31" s="47"/>
       <c r="H31" s="6" t="s">
         <v>56</v>
       </c>
@@ -2849,13 +2855,13 @@
       <c r="L31" s="39">
         <v>60634.099956999999</v>
       </c>
-      <c r="M31" s="40">
+      <c r="M31" s="41">
         <v>34.7914076844351</v>
       </c>
-      <c r="N31" s="40">
+      <c r="N31" s="41">
         <v>34.400796508789099</v>
       </c>
-      <c r="O31" s="40">
+      <c r="O31" s="41">
         <v>35.0925380706787</v>
       </c>
       <c r="P31" s="39">
@@ -2869,12 +2875,12 @@
       </c>
     </row>
     <row r="32" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B32" s="41"/>
-      <c r="C32" s="41"/>
-      <c r="D32" s="42"/>
-      <c r="E32" s="43"/>
-      <c r="F32" s="44"/>
-      <c r="G32" s="43"/>
+      <c r="B32" s="46"/>
+      <c r="C32" s="46"/>
+      <c r="D32" s="50"/>
+      <c r="E32" s="47"/>
+      <c r="F32" s="48"/>
+      <c r="G32" s="47"/>
       <c r="H32" s="6" t="s">
         <v>199</v>
       </c>
@@ -2886,20 +2892,20 @@
       </c>
       <c r="K32" s="6"/>
       <c r="L32" s="39"/>
-      <c r="M32" s="40"/>
-      <c r="N32" s="40"/>
-      <c r="O32" s="40"/>
+      <c r="M32" s="41"/>
+      <c r="N32" s="41"/>
+      <c r="O32" s="41"/>
       <c r="P32" s="39"/>
       <c r="Q32" s="39"/>
       <c r="R32" s="39"/>
     </row>
     <row r="33" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B33" s="41"/>
-      <c r="C33" s="41"/>
-      <c r="D33" s="42"/>
-      <c r="E33" s="43"/>
-      <c r="F33" s="44"/>
-      <c r="G33" s="43"/>
+      <c r="B33" s="46"/>
+      <c r="C33" s="46"/>
+      <c r="D33" s="50"/>
+      <c r="E33" s="47"/>
+      <c r="F33" s="48"/>
+      <c r="G33" s="47"/>
       <c r="H33" s="6" t="s">
         <v>182</v>
       </c>
@@ -2909,20 +2915,20 @@
       <c r="J33" s="6"/>
       <c r="K33" s="6"/>
       <c r="L33" s="39"/>
-      <c r="M33" s="40"/>
-      <c r="N33" s="40"/>
-      <c r="O33" s="40"/>
+      <c r="M33" s="41"/>
+      <c r="N33" s="41"/>
+      <c r="O33" s="41"/>
       <c r="P33" s="39"/>
       <c r="Q33" s="39"/>
       <c r="R33" s="39"/>
     </row>
     <row r="34" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B34" s="41"/>
-      <c r="C34" s="41"/>
-      <c r="D34" s="42"/>
-      <c r="E34" s="43"/>
-      <c r="F34" s="44"/>
-      <c r="G34" s="43"/>
+      <c r="B34" s="46"/>
+      <c r="C34" s="46"/>
+      <c r="D34" s="50"/>
+      <c r="E34" s="47"/>
+      <c r="F34" s="48"/>
+      <c r="G34" s="47"/>
       <c r="H34" s="6" t="s">
         <v>107</v>
       </c>
@@ -2932,30 +2938,30 @@
       <c r="J34" s="6"/>
       <c r="K34" s="6"/>
       <c r="L34" s="39"/>
-      <c r="M34" s="40"/>
-      <c r="N34" s="40"/>
-      <c r="O34" s="40"/>
+      <c r="M34" s="41"/>
+      <c r="N34" s="41"/>
+      <c r="O34" s="41"/>
       <c r="P34" s="39"/>
       <c r="Q34" s="39"/>
       <c r="R34" s="39"/>
     </row>
     <row r="35" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B35" s="41" t="s">
+      <c r="B35" s="46" t="s">
         <v>67</v>
       </c>
-      <c r="C35" s="41" t="s">
+      <c r="C35" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="D35" s="42" t="s">
+      <c r="D35" s="50" t="s">
         <v>149</v>
       </c>
-      <c r="E35" s="42" t="s">
+      <c r="E35" s="50" t="s">
         <v>186</v>
       </c>
-      <c r="F35" s="44" t="s">
+      <c r="F35" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="G35" s="43" t="s">
+      <c r="G35" s="47" t="s">
         <v>185</v>
       </c>
       <c r="H35" s="6" t="s">
@@ -2967,13 +2973,13 @@
       <c r="L35" s="39">
         <v>7836.9224329999997</v>
       </c>
-      <c r="M35" s="40">
+      <c r="M35" s="41">
         <v>30.812020422114401</v>
       </c>
-      <c r="N35" s="40">
+      <c r="N35" s="41">
         <v>29.280075073242202</v>
       </c>
-      <c r="O35" s="40">
+      <c r="O35" s="41">
         <v>32.002838897705097</v>
       </c>
       <c r="P35" s="39">
@@ -2987,12 +2993,12 @@
       </c>
     </row>
     <row r="36" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B36" s="41"/>
-      <c r="C36" s="41"/>
-      <c r="D36" s="42"/>
-      <c r="E36" s="42"/>
-      <c r="F36" s="44"/>
-      <c r="G36" s="43"/>
+      <c r="B36" s="46"/>
+      <c r="C36" s="46"/>
+      <c r="D36" s="50"/>
+      <c r="E36" s="50"/>
+      <c r="F36" s="48"/>
+      <c r="G36" s="47"/>
       <c r="H36" s="6" t="s">
         <v>51</v>
       </c>
@@ -3002,20 +3008,20 @@
       <c r="J36" s="6"/>
       <c r="K36" s="6"/>
       <c r="L36" s="39"/>
-      <c r="M36" s="40"/>
-      <c r="N36" s="40"/>
-      <c r="O36" s="40"/>
+      <c r="M36" s="41"/>
+      <c r="N36" s="41"/>
+      <c r="O36" s="41"/>
       <c r="P36" s="39"/>
       <c r="Q36" s="39"/>
       <c r="R36" s="39"/>
     </row>
     <row r="37" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B37" s="41"/>
-      <c r="C37" s="41"/>
-      <c r="D37" s="42"/>
-      <c r="E37" s="42"/>
-      <c r="F37" s="44"/>
-      <c r="G37" s="43"/>
+      <c r="B37" s="46"/>
+      <c r="C37" s="46"/>
+      <c r="D37" s="50"/>
+      <c r="E37" s="50"/>
+      <c r="F37" s="48"/>
+      <c r="G37" s="47"/>
       <c r="H37" s="6" t="s">
         <v>69</v>
       </c>
@@ -3025,30 +3031,30 @@
       <c r="J37" s="6"/>
       <c r="K37" s="6"/>
       <c r="L37" s="39"/>
-      <c r="M37" s="40"/>
-      <c r="N37" s="40"/>
-      <c r="O37" s="40"/>
+      <c r="M37" s="41"/>
+      <c r="N37" s="41"/>
+      <c r="O37" s="41"/>
       <c r="P37" s="39"/>
       <c r="Q37" s="39"/>
       <c r="R37" s="39"/>
     </row>
     <row r="38" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B38" s="41" t="s">
+      <c r="B38" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="C38" s="41" t="s">
+      <c r="C38" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="D38" s="42" t="s">
+      <c r="D38" s="50" t="s">
         <v>155</v>
       </c>
-      <c r="E38" s="42" t="s">
+      <c r="E38" s="50" t="s">
         <v>187</v>
       </c>
-      <c r="F38" s="44" t="s">
+      <c r="F38" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="G38" s="43" t="s">
+      <c r="G38" s="47" t="s">
         <v>185</v>
       </c>
       <c r="H38" s="6" t="s">
@@ -3062,13 +3068,13 @@
       <c r="L38" s="39">
         <v>1445.132656</v>
       </c>
-      <c r="M38" s="40">
+      <c r="M38" s="41">
         <v>31.446646721207401</v>
       </c>
-      <c r="N38" s="40">
+      <c r="N38" s="41">
         <v>30.847949218749999</v>
       </c>
-      <c r="O38" s="40">
+      <c r="O38" s="41">
         <v>31.925752639770501</v>
       </c>
       <c r="P38" s="39">
@@ -3082,12 +3088,12 @@
       </c>
     </row>
     <row r="39" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B39" s="41"/>
-      <c r="C39" s="41"/>
-      <c r="D39" s="42"/>
-      <c r="E39" s="42"/>
-      <c r="F39" s="44"/>
-      <c r="G39" s="43"/>
+      <c r="B39" s="46"/>
+      <c r="C39" s="46"/>
+      <c r="D39" s="50"/>
+      <c r="E39" s="50"/>
+      <c r="F39" s="48"/>
+      <c r="G39" s="47"/>
       <c r="H39" s="6" t="s">
         <v>184</v>
       </c>
@@ -3097,30 +3103,30 @@
       <c r="J39" s="6"/>
       <c r="K39" s="6"/>
       <c r="L39" s="39"/>
-      <c r="M39" s="40"/>
-      <c r="N39" s="40"/>
-      <c r="O39" s="40"/>
+      <c r="M39" s="41"/>
+      <c r="N39" s="41"/>
+      <c r="O39" s="41"/>
       <c r="P39" s="39"/>
       <c r="Q39" s="39"/>
       <c r="R39" s="39"/>
     </row>
     <row r="40" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B40" s="41" t="s">
+      <c r="B40" s="46" t="s">
         <v>182</v>
       </c>
-      <c r="C40" s="41" t="s">
+      <c r="C40" s="46" t="s">
         <v>156</v>
       </c>
-      <c r="D40" s="42" t="s">
+      <c r="D40" s="50" t="s">
         <v>155</v>
       </c>
-      <c r="E40" s="43" t="s">
+      <c r="E40" s="47" t="s">
         <v>240</v>
       </c>
-      <c r="F40" s="46" t="s">
+      <c r="F40" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="G40" s="43"/>
+      <c r="G40" s="47"/>
       <c r="H40" s="6" t="s">
         <v>200</v>
       </c>
@@ -3132,13 +3138,13 @@
       <c r="L40" s="39">
         <v>4554.17461</v>
       </c>
-      <c r="M40" s="40">
+      <c r="M40" s="41">
         <v>33.414820649644497</v>
       </c>
-      <c r="N40" s="40">
+      <c r="N40" s="41">
         <v>32.605027770996102</v>
       </c>
-      <c r="O40" s="40">
+      <c r="O40" s="41">
         <v>33.992408752441399</v>
       </c>
       <c r="P40" s="39">
@@ -3152,12 +3158,12 @@
       </c>
     </row>
     <row r="41" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B41" s="41"/>
-      <c r="C41" s="41"/>
-      <c r="D41" s="42"/>
-      <c r="E41" s="43"/>
-      <c r="F41" s="46"/>
-      <c r="G41" s="43"/>
+      <c r="B41" s="46"/>
+      <c r="C41" s="46"/>
+      <c r="D41" s="50"/>
+      <c r="E41" s="47"/>
+      <c r="F41" s="49"/>
+      <c r="G41" s="47"/>
       <c r="H41" s="6" t="s">
         <v>65</v>
       </c>
@@ -3167,9 +3173,9 @@
       <c r="J41" s="6"/>
       <c r="K41" s="6"/>
       <c r="L41" s="39"/>
-      <c r="M41" s="40"/>
-      <c r="N41" s="40"/>
-      <c r="O41" s="40"/>
+      <c r="M41" s="41"/>
+      <c r="N41" s="41"/>
+      <c r="O41" s="41"/>
       <c r="P41" s="39"/>
       <c r="Q41" s="39"/>
       <c r="R41" s="39"/>
@@ -3267,22 +3273,22 @@
       </c>
     </row>
     <row r="44" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B44" s="41" t="s">
+      <c r="B44" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="C44" s="41" t="s">
+      <c r="C44" s="46" t="s">
         <v>78</v>
       </c>
-      <c r="D44" s="42" t="s">
+      <c r="D44" s="50" t="s">
         <v>134</v>
       </c>
-      <c r="E44" s="42" t="s">
+      <c r="E44" s="50" t="s">
         <v>159</v>
       </c>
-      <c r="F44" s="44" t="s">
+      <c r="F44" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="G44" s="43"/>
+      <c r="G44" s="47"/>
       <c r="H44" s="6" t="s">
         <v>11</v>
       </c>
@@ -3294,13 +3300,13 @@
       <c r="L44" s="39">
         <v>21007.8607271</v>
       </c>
-      <c r="M44" s="40">
+      <c r="M44" s="41">
         <v>34.942636835841803</v>
       </c>
-      <c r="N44" s="40">
+      <c r="N44" s="41">
         <v>34.706142425537102</v>
       </c>
-      <c r="O44" s="40">
+      <c r="O44" s="41">
         <v>35.1235160827637</v>
       </c>
       <c r="P44" s="39">
@@ -3314,12 +3320,12 @@
       </c>
     </row>
     <row r="45" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B45" s="41"/>
-      <c r="C45" s="41"/>
-      <c r="D45" s="42"/>
-      <c r="E45" s="42"/>
-      <c r="F45" s="44"/>
-      <c r="G45" s="43"/>
+      <c r="B45" s="46"/>
+      <c r="C45" s="46"/>
+      <c r="D45" s="50"/>
+      <c r="E45" s="50"/>
+      <c r="F45" s="48"/>
+      <c r="G45" s="47"/>
       <c r="H45" s="6" t="s">
         <v>17</v>
       </c>
@@ -3329,20 +3335,20 @@
       <c r="J45" s="6"/>
       <c r="K45" s="6"/>
       <c r="L45" s="39"/>
-      <c r="M45" s="40"/>
-      <c r="N45" s="40"/>
-      <c r="O45" s="40"/>
+      <c r="M45" s="41"/>
+      <c r="N45" s="41"/>
+      <c r="O45" s="41"/>
       <c r="P45" s="39"/>
       <c r="Q45" s="39"/>
       <c r="R45" s="39"/>
     </row>
     <row r="46" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B46" s="41"/>
-      <c r="C46" s="41"/>
-      <c r="D46" s="42"/>
-      <c r="E46" s="42"/>
-      <c r="F46" s="44"/>
-      <c r="G46" s="43"/>
+      <c r="B46" s="46"/>
+      <c r="C46" s="46"/>
+      <c r="D46" s="50"/>
+      <c r="E46" s="50"/>
+      <c r="F46" s="48"/>
+      <c r="G46" s="47"/>
       <c r="H46" s="6" t="s">
         <v>74</v>
       </c>
@@ -3354,9 +3360,9 @@
         <v>180</v>
       </c>
       <c r="L46" s="39"/>
-      <c r="M46" s="40"/>
-      <c r="N46" s="40"/>
-      <c r="O46" s="40"/>
+      <c r="M46" s="41"/>
+      <c r="N46" s="41"/>
+      <c r="O46" s="41"/>
       <c r="P46" s="39"/>
       <c r="Q46" s="39"/>
       <c r="R46" s="39"/>
@@ -3413,20 +3419,20 @@
       </c>
     </row>
     <row r="48" spans="2:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="B48" s="41" t="s">
+      <c r="B48" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="C48" s="41" t="s">
+      <c r="C48" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="D48" s="42" t="s">
+      <c r="D48" s="50" t="s">
         <v>150</v>
       </c>
-      <c r="E48" s="44"/>
-      <c r="F48" s="44" t="s">
+      <c r="E48" s="48"/>
+      <c r="F48" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="G48" s="43" t="s">
+      <c r="G48" s="47" t="s">
         <v>88</v>
       </c>
       <c r="H48" s="6" t="s">
@@ -3437,35 +3443,35 @@
       </c>
       <c r="J48" s="6"/>
       <c r="K48" s="6"/>
-      <c r="L48" s="50">
+      <c r="L48" s="43">
         <v>73500.915290000004</v>
       </c>
-      <c r="M48" s="52">
+      <c r="M48" s="45">
         <v>35.320639295166302</v>
       </c>
-      <c r="N48" s="52">
+      <c r="N48" s="45">
         <v>35.1950874328613</v>
       </c>
-      <c r="O48" s="52">
+      <c r="O48" s="45">
         <v>35.432624816894503</v>
       </c>
-      <c r="P48" s="50">
+      <c r="P48" s="43">
         <v>138.30608005498701</v>
       </c>
-      <c r="Q48" s="50">
+      <c r="Q48" s="43">
         <v>87.567283630371094</v>
       </c>
-      <c r="R48" s="50">
+      <c r="R48" s="43">
         <v>176.65103149414099</v>
       </c>
     </row>
     <row r="49" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B49" s="41"/>
-      <c r="C49" s="41"/>
-      <c r="D49" s="42"/>
-      <c r="E49" s="44"/>
-      <c r="F49" s="44"/>
-      <c r="G49" s="43"/>
+      <c r="B49" s="46"/>
+      <c r="C49" s="46"/>
+      <c r="D49" s="50"/>
+      <c r="E49" s="48"/>
+      <c r="F49" s="48"/>
+      <c r="G49" s="47"/>
       <c r="H49" s="6" t="s">
         <v>11</v>
       </c>
@@ -3474,29 +3480,29 @@
       </c>
       <c r="J49" s="6"/>
       <c r="K49" s="6"/>
-      <c r="L49" s="51"/>
-      <c r="M49" s="51"/>
-      <c r="N49" s="51"/>
-      <c r="O49" s="51"/>
-      <c r="P49" s="51"/>
-      <c r="Q49" s="51"/>
-      <c r="R49" s="51"/>
+      <c r="L49" s="44"/>
+      <c r="M49" s="44"/>
+      <c r="N49" s="44"/>
+      <c r="O49" s="44"/>
+      <c r="P49" s="44"/>
+      <c r="Q49" s="44"/>
+      <c r="R49" s="44"/>
     </row>
     <row r="50" spans="2:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="B50" s="41" t="s">
+      <c r="B50" s="46" t="s">
         <v>89</v>
       </c>
-      <c r="C50" s="41" t="s">
+      <c r="C50" s="46" t="s">
         <v>91</v>
       </c>
-      <c r="D50" s="42" t="s">
+      <c r="D50" s="50" t="s">
         <v>162</v>
       </c>
-      <c r="E50" s="44"/>
-      <c r="F50" s="44" t="s">
+      <c r="E50" s="48"/>
+      <c r="F50" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="G50" s="43" t="s">
+      <c r="G50" s="47" t="s">
         <v>88</v>
       </c>
       <c r="H50" s="6" t="s">
@@ -3510,13 +3516,13 @@
       <c r="L50" s="39">
         <v>26517.169783000001</v>
       </c>
-      <c r="M50" s="40">
+      <c r="M50" s="41">
         <v>35.107022147221301</v>
       </c>
-      <c r="N50" s="40">
+      <c r="N50" s="41">
         <v>34.843528747558601</v>
       </c>
-      <c r="O50" s="40">
+      <c r="O50" s="41">
         <v>35.256871032714798</v>
       </c>
       <c r="P50" s="39">
@@ -3530,12 +3536,12 @@
       </c>
     </row>
     <row r="51" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B51" s="41"/>
-      <c r="C51" s="41"/>
-      <c r="D51" s="42"/>
-      <c r="E51" s="44"/>
-      <c r="F51" s="44"/>
-      <c r="G51" s="43"/>
+      <c r="B51" s="46"/>
+      <c r="C51" s="46"/>
+      <c r="D51" s="50"/>
+      <c r="E51" s="48"/>
+      <c r="F51" s="48"/>
+      <c r="G51" s="47"/>
       <c r="H51" s="6" t="s">
         <v>191</v>
       </c>
@@ -3545,20 +3551,20 @@
       <c r="J51" s="6"/>
       <c r="K51" s="6"/>
       <c r="L51" s="39"/>
-      <c r="M51" s="40"/>
-      <c r="N51" s="40"/>
-      <c r="O51" s="40"/>
+      <c r="M51" s="41"/>
+      <c r="N51" s="41"/>
+      <c r="O51" s="41"/>
       <c r="P51" s="39"/>
       <c r="Q51" s="39"/>
       <c r="R51" s="39"/>
     </row>
     <row r="52" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B52" s="41"/>
-      <c r="C52" s="41"/>
-      <c r="D52" s="42"/>
-      <c r="E52" s="44"/>
-      <c r="F52" s="44"/>
-      <c r="G52" s="43"/>
+      <c r="B52" s="46"/>
+      <c r="C52" s="46"/>
+      <c r="D52" s="50"/>
+      <c r="E52" s="48"/>
+      <c r="F52" s="48"/>
+      <c r="G52" s="47"/>
       <c r="H52" s="6" t="s">
         <v>107</v>
       </c>
@@ -3568,30 +3574,30 @@
       <c r="J52" s="6"/>
       <c r="K52" s="6"/>
       <c r="L52" s="39"/>
-      <c r="M52" s="40"/>
-      <c r="N52" s="40"/>
-      <c r="O52" s="40"/>
+      <c r="M52" s="41"/>
+      <c r="N52" s="41"/>
+      <c r="O52" s="41"/>
       <c r="P52" s="39"/>
       <c r="Q52" s="39"/>
       <c r="R52" s="39"/>
     </row>
     <row r="53" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B53" s="41" t="s">
+      <c r="B53" s="46" t="s">
         <v>92</v>
       </c>
-      <c r="C53" s="41" t="s">
+      <c r="C53" s="46" t="s">
         <v>93</v>
       </c>
-      <c r="D53" s="42" t="s">
+      <c r="D53" s="50" t="s">
         <v>162</v>
       </c>
-      <c r="E53" s="43" t="s">
+      <c r="E53" s="47" t="s">
         <v>161</v>
       </c>
-      <c r="F53" s="44" t="s">
+      <c r="F53" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="G53" s="43" t="s">
+      <c r="G53" s="47" t="s">
         <v>14</v>
       </c>
       <c r="H53" s="6" t="s">
@@ -3605,13 +3611,13 @@
       <c r="L53" s="39">
         <v>32689.860002000001</v>
       </c>
-      <c r="M53" s="40">
+      <c r="M53" s="41">
         <v>33.658222219683701</v>
       </c>
-      <c r="N53" s="40">
+      <c r="N53" s="41">
         <v>32.644596099853501</v>
       </c>
-      <c r="O53" s="40">
+      <c r="O53" s="41">
         <v>34.228927612304702</v>
       </c>
       <c r="P53" s="39">
@@ -3625,12 +3631,12 @@
       </c>
     </row>
     <row r="54" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B54" s="41"/>
-      <c r="C54" s="41"/>
-      <c r="D54" s="42"/>
-      <c r="E54" s="43"/>
-      <c r="F54" s="44"/>
-      <c r="G54" s="43"/>
+      <c r="B54" s="46"/>
+      <c r="C54" s="46"/>
+      <c r="D54" s="50"/>
+      <c r="E54" s="47"/>
+      <c r="F54" s="48"/>
+      <c r="G54" s="47"/>
       <c r="H54" s="6" t="s">
         <v>34</v>
       </c>
@@ -3640,20 +3646,20 @@
       <c r="J54" s="6"/>
       <c r="K54" s="6"/>
       <c r="L54" s="39"/>
-      <c r="M54" s="40"/>
-      <c r="N54" s="40"/>
-      <c r="O54" s="40"/>
+      <c r="M54" s="41"/>
+      <c r="N54" s="41"/>
+      <c r="O54" s="41"/>
       <c r="P54" s="39"/>
       <c r="Q54" s="39"/>
       <c r="R54" s="39"/>
     </row>
     <row r="55" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B55" s="41"/>
-      <c r="C55" s="41"/>
-      <c r="D55" s="42"/>
-      <c r="E55" s="43"/>
-      <c r="F55" s="44"/>
-      <c r="G55" s="43"/>
+      <c r="B55" s="46"/>
+      <c r="C55" s="46"/>
+      <c r="D55" s="50"/>
+      <c r="E55" s="47"/>
+      <c r="F55" s="48"/>
+      <c r="G55" s="47"/>
       <c r="H55" s="6" t="s">
         <v>17</v>
       </c>
@@ -3663,20 +3669,20 @@
       <c r="J55" s="6"/>
       <c r="K55" s="6"/>
       <c r="L55" s="39"/>
-      <c r="M55" s="40"/>
-      <c r="N55" s="40"/>
-      <c r="O55" s="40"/>
+      <c r="M55" s="41"/>
+      <c r="N55" s="41"/>
+      <c r="O55" s="41"/>
       <c r="P55" s="39"/>
       <c r="Q55" s="39"/>
       <c r="R55" s="39"/>
     </row>
     <row r="56" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B56" s="41"/>
-      <c r="C56" s="41"/>
-      <c r="D56" s="42"/>
-      <c r="E56" s="43"/>
-      <c r="F56" s="44"/>
-      <c r="G56" s="43"/>
+      <c r="B56" s="46"/>
+      <c r="C56" s="46"/>
+      <c r="D56" s="50"/>
+      <c r="E56" s="47"/>
+      <c r="F56" s="48"/>
+      <c r="G56" s="47"/>
       <c r="H56" s="18" t="s">
         <v>117</v>
       </c>
@@ -3686,9 +3692,9 @@
       <c r="J56" s="6"/>
       <c r="K56" s="6"/>
       <c r="L56" s="39"/>
-      <c r="M56" s="40"/>
-      <c r="N56" s="40"/>
-      <c r="O56" s="40"/>
+      <c r="M56" s="41"/>
+      <c r="N56" s="41"/>
+      <c r="O56" s="41"/>
       <c r="P56" s="39"/>
       <c r="Q56" s="39"/>
       <c r="R56" s="39"/>
@@ -3888,22 +3894,22 @@
       </c>
     </row>
     <row r="61" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B61" s="41" t="s">
+      <c r="B61" s="46" t="s">
         <v>105</v>
       </c>
-      <c r="C61" s="41" t="s">
+      <c r="C61" s="46" t="s">
         <v>106</v>
       </c>
-      <c r="D61" s="42" t="s">
+      <c r="D61" s="50" t="s">
         <v>164</v>
       </c>
-      <c r="E61" s="43" t="s">
+      <c r="E61" s="47" t="s">
         <v>193</v>
       </c>
-      <c r="F61" s="44" t="s">
+      <c r="F61" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="G61" s="43" t="s">
+      <c r="G61" s="47" t="s">
         <v>185</v>
       </c>
       <c r="H61" s="6" t="s">
@@ -3917,13 +3923,13 @@
       <c r="L61" s="39">
         <v>205.69440399999999</v>
       </c>
-      <c r="M61" s="40">
+      <c r="M61" s="41">
         <v>29.280778035250599</v>
       </c>
-      <c r="N61" s="40">
+      <c r="N61" s="41">
         <v>26.6988620758057</v>
       </c>
-      <c r="O61" s="40">
+      <c r="O61" s="41">
         <v>31.488284683227501</v>
       </c>
       <c r="P61" s="39">
@@ -3937,12 +3943,12 @@
       </c>
     </row>
     <row r="62" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B62" s="41"/>
-      <c r="C62" s="41"/>
-      <c r="D62" s="42"/>
-      <c r="E62" s="43"/>
-      <c r="F62" s="44"/>
-      <c r="G62" s="43"/>
+      <c r="B62" s="46"/>
+      <c r="C62" s="46"/>
+      <c r="D62" s="50"/>
+      <c r="E62" s="47"/>
+      <c r="F62" s="48"/>
+      <c r="G62" s="47"/>
       <c r="H62" s="6" t="s">
         <v>28</v>
       </c>
@@ -3952,30 +3958,30 @@
       <c r="J62" s="6"/>
       <c r="K62" s="6"/>
       <c r="L62" s="39"/>
-      <c r="M62" s="40"/>
-      <c r="N62" s="40"/>
-      <c r="O62" s="40"/>
+      <c r="M62" s="41"/>
+      <c r="N62" s="41"/>
+      <c r="O62" s="41"/>
       <c r="P62" s="39"/>
       <c r="Q62" s="39"/>
       <c r="R62" s="39"/>
     </row>
     <row r="63" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B63" s="41" t="s">
+      <c r="B63" s="46" t="s">
         <v>107</v>
       </c>
-      <c r="C63" s="41" t="s">
+      <c r="C63" s="46" t="s">
         <v>108</v>
       </c>
-      <c r="D63" s="42" t="s">
+      <c r="D63" s="50" t="s">
         <v>175</v>
       </c>
-      <c r="E63" s="44" t="s">
+      <c r="E63" s="48" t="s">
         <v>174</v>
       </c>
-      <c r="F63" s="44" t="s">
+      <c r="F63" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="G63" s="43"/>
+      <c r="G63" s="47"/>
       <c r="H63" s="6" t="s">
         <v>56</v>
       </c>
@@ -3987,13 +3993,13 @@
       <c r="L63" s="39">
         <v>264252.94453600002</v>
       </c>
-      <c r="M63" s="40">
+      <c r="M63" s="41">
         <v>35.033322022745303</v>
       </c>
-      <c r="N63" s="40">
+      <c r="N63" s="41">
         <v>34.782768249511697</v>
       </c>
-      <c r="O63" s="40">
+      <c r="O63" s="41">
         <v>35.230577850341803</v>
       </c>
       <c r="P63" s="39">
@@ -4007,12 +4013,12 @@
       </c>
     </row>
     <row r="64" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B64" s="41"/>
-      <c r="C64" s="41"/>
-      <c r="D64" s="42"/>
-      <c r="E64" s="44"/>
-      <c r="F64" s="44"/>
-      <c r="G64" s="43"/>
+      <c r="B64" s="46"/>
+      <c r="C64" s="46"/>
+      <c r="D64" s="50"/>
+      <c r="E64" s="48"/>
+      <c r="F64" s="48"/>
+      <c r="G64" s="47"/>
       <c r="H64" s="6" t="s">
         <v>109</v>
       </c>
@@ -4022,20 +4028,20 @@
       <c r="J64" s="6"/>
       <c r="K64" s="6"/>
       <c r="L64" s="39"/>
-      <c r="M64" s="40"/>
-      <c r="N64" s="40"/>
-      <c r="O64" s="40"/>
+      <c r="M64" s="41"/>
+      <c r="N64" s="41"/>
+      <c r="O64" s="41"/>
       <c r="P64" s="39"/>
       <c r="Q64" s="39"/>
       <c r="R64" s="39"/>
     </row>
     <row r="65" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B65" s="41"/>
-      <c r="C65" s="41"/>
-      <c r="D65" s="42"/>
-      <c r="E65" s="44"/>
-      <c r="F65" s="44"/>
-      <c r="G65" s="43"/>
+      <c r="B65" s="46"/>
+      <c r="C65" s="46"/>
+      <c r="D65" s="50"/>
+      <c r="E65" s="48"/>
+      <c r="F65" s="48"/>
+      <c r="G65" s="47"/>
       <c r="H65" s="6" t="s">
         <v>11</v>
       </c>
@@ -4045,20 +4051,20 @@
       <c r="J65" s="6"/>
       <c r="K65" s="6"/>
       <c r="L65" s="39"/>
-      <c r="M65" s="40"/>
-      <c r="N65" s="40"/>
-      <c r="O65" s="40"/>
+      <c r="M65" s="41"/>
+      <c r="N65" s="41"/>
+      <c r="O65" s="41"/>
       <c r="P65" s="39"/>
       <c r="Q65" s="39"/>
       <c r="R65" s="39"/>
     </row>
     <row r="66" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B66" s="41"/>
-      <c r="C66" s="41"/>
-      <c r="D66" s="42"/>
-      <c r="E66" s="44"/>
-      <c r="F66" s="44"/>
-      <c r="G66" s="43"/>
+      <c r="B66" s="46"/>
+      <c r="C66" s="46"/>
+      <c r="D66" s="50"/>
+      <c r="E66" s="48"/>
+      <c r="F66" s="48"/>
+      <c r="G66" s="47"/>
       <c r="H66" s="6" t="s">
         <v>65</v>
       </c>
@@ -4068,20 +4074,20 @@
       <c r="J66" s="6"/>
       <c r="K66" s="6"/>
       <c r="L66" s="39"/>
-      <c r="M66" s="40"/>
-      <c r="N66" s="40"/>
-      <c r="O66" s="40"/>
+      <c r="M66" s="41"/>
+      <c r="N66" s="41"/>
+      <c r="O66" s="41"/>
       <c r="P66" s="39"/>
       <c r="Q66" s="39"/>
       <c r="R66" s="39"/>
     </row>
     <row r="67" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B67" s="41"/>
-      <c r="C67" s="41"/>
-      <c r="D67" s="42"/>
-      <c r="E67" s="44"/>
-      <c r="F67" s="44"/>
-      <c r="G67" s="43"/>
+      <c r="B67" s="46"/>
+      <c r="C67" s="46"/>
+      <c r="D67" s="50"/>
+      <c r="E67" s="48"/>
+      <c r="F67" s="48"/>
+      <c r="G67" s="47"/>
       <c r="H67" s="6" t="s">
         <v>28</v>
       </c>
@@ -4091,20 +4097,20 @@
       <c r="J67" s="6"/>
       <c r="K67" s="6"/>
       <c r="L67" s="39"/>
-      <c r="M67" s="40"/>
-      <c r="N67" s="40"/>
-      <c r="O67" s="40"/>
+      <c r="M67" s="41"/>
+      <c r="N67" s="41"/>
+      <c r="O67" s="41"/>
       <c r="P67" s="39"/>
       <c r="Q67" s="39"/>
       <c r="R67" s="39"/>
     </row>
     <row r="68" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B68" s="41"/>
-      <c r="C68" s="41"/>
-      <c r="D68" s="42"/>
-      <c r="E68" s="44"/>
-      <c r="F68" s="44"/>
-      <c r="G68" s="43"/>
+      <c r="B68" s="46"/>
+      <c r="C68" s="46"/>
+      <c r="D68" s="50"/>
+      <c r="E68" s="48"/>
+      <c r="F68" s="48"/>
+      <c r="G68" s="47"/>
       <c r="H68" s="6" t="s">
         <v>197</v>
       </c>
@@ -4114,20 +4120,20 @@
       <c r="J68" s="6"/>
       <c r="K68" s="6"/>
       <c r="L68" s="39"/>
-      <c r="M68" s="40"/>
-      <c r="N68" s="40"/>
-      <c r="O68" s="40"/>
+      <c r="M68" s="41"/>
+      <c r="N68" s="41"/>
+      <c r="O68" s="41"/>
       <c r="P68" s="39"/>
       <c r="Q68" s="39"/>
       <c r="R68" s="39"/>
     </row>
     <row r="69" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B69" s="41"/>
-      <c r="C69" s="41"/>
-      <c r="D69" s="42"/>
-      <c r="E69" s="44"/>
-      <c r="F69" s="44"/>
-      <c r="G69" s="43"/>
+      <c r="B69" s="46"/>
+      <c r="C69" s="46"/>
+      <c r="D69" s="50"/>
+      <c r="E69" s="48"/>
+      <c r="F69" s="48"/>
+      <c r="G69" s="47"/>
       <c r="H69" s="6" t="s">
         <v>63</v>
       </c>
@@ -4137,9 +4143,9 @@
       <c r="J69" s="6"/>
       <c r="K69" s="6"/>
       <c r="L69" s="39"/>
-      <c r="M69" s="40"/>
-      <c r="N69" s="40"/>
-      <c r="O69" s="40"/>
+      <c r="M69" s="41"/>
+      <c r="N69" s="41"/>
+      <c r="O69" s="41"/>
       <c r="P69" s="39"/>
       <c r="Q69" s="39"/>
       <c r="R69" s="39"/>
@@ -4192,22 +4198,22 @@
       </c>
     </row>
     <row r="71" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B71" s="41" t="s">
+      <c r="B71" s="46" t="s">
         <v>111</v>
       </c>
-      <c r="C71" s="41" t="s">
+      <c r="C71" s="46" t="s">
         <v>112</v>
       </c>
-      <c r="D71" s="42" t="s">
+      <c r="D71" s="50" t="s">
         <v>164</v>
       </c>
-      <c r="E71" s="43" t="s">
+      <c r="E71" s="47" t="s">
         <v>166</v>
       </c>
-      <c r="F71" s="44" t="s">
+      <c r="F71" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="G71" s="43" t="s">
+      <c r="G71" s="47" t="s">
         <v>185</v>
       </c>
       <c r="H71" s="6" t="s">
@@ -4221,13 +4227,13 @@
       <c r="L71" s="39">
         <v>2278.6253320000001</v>
       </c>
-      <c r="M71" s="40">
+      <c r="M71" s="41">
         <v>31.040425460681899</v>
       </c>
-      <c r="N71" s="40">
+      <c r="N71" s="41">
         <v>29.9775085449219</v>
       </c>
-      <c r="O71" s="40">
+      <c r="O71" s="41">
         <v>31.896238327026399</v>
       </c>
       <c r="P71" s="39">
@@ -4241,12 +4247,12 @@
       </c>
     </row>
     <row r="72" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B72" s="41"/>
-      <c r="C72" s="41"/>
-      <c r="D72" s="42"/>
-      <c r="E72" s="43"/>
-      <c r="F72" s="44"/>
-      <c r="G72" s="43"/>
+      <c r="B72" s="46"/>
+      <c r="C72" s="46"/>
+      <c r="D72" s="50"/>
+      <c r="E72" s="47"/>
+      <c r="F72" s="48"/>
+      <c r="G72" s="47"/>
       <c r="H72" s="6" t="s">
         <v>28</v>
       </c>
@@ -4256,9 +4262,9 @@
       <c r="J72" s="6"/>
       <c r="K72" s="6"/>
       <c r="L72" s="39"/>
-      <c r="M72" s="40"/>
-      <c r="N72" s="40"/>
-      <c r="O72" s="40"/>
+      <c r="M72" s="41"/>
+      <c r="N72" s="41"/>
+      <c r="O72" s="41"/>
       <c r="P72" s="39"/>
       <c r="Q72" s="39"/>
       <c r="R72" s="39"/>
@@ -4313,22 +4319,22 @@
       </c>
     </row>
     <row r="74" spans="2:18" ht="72.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="41" t="s">
+      <c r="B74" s="46" t="s">
         <v>115</v>
       </c>
-      <c r="C74" s="41" t="s">
+      <c r="C74" s="46" t="s">
         <v>116</v>
       </c>
-      <c r="D74" s="42" t="s">
+      <c r="D74" s="50" t="s">
         <v>164</v>
       </c>
-      <c r="E74" s="47" t="s">
+      <c r="E74" s="51" t="s">
         <v>167</v>
       </c>
-      <c r="F74" s="44" t="s">
+      <c r="F74" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="G74" s="43" t="s">
+      <c r="G74" s="47" t="s">
         <v>196</v>
       </c>
       <c r="H74" s="6" t="s">
@@ -4342,13 +4348,13 @@
       <c r="L74" s="39">
         <v>95.092663999999999</v>
       </c>
-      <c r="M74" s="40">
+      <c r="M74" s="41">
         <v>30.928038921171002</v>
       </c>
-      <c r="N74" s="40">
+      <c r="N74" s="41">
         <v>29.6979766845703</v>
       </c>
-      <c r="O74" s="40">
+      <c r="O74" s="41">
         <v>31.8562515258789</v>
       </c>
       <c r="P74" s="39">
@@ -4362,12 +4368,12 @@
       </c>
     </row>
     <row r="75" spans="2:18" ht="72.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="41"/>
-      <c r="C75" s="41"/>
-      <c r="D75" s="42"/>
-      <c r="E75" s="47"/>
-      <c r="F75" s="44"/>
-      <c r="G75" s="43"/>
+      <c r="B75" s="46"/>
+      <c r="C75" s="46"/>
+      <c r="D75" s="50"/>
+      <c r="E75" s="51"/>
+      <c r="F75" s="48"/>
+      <c r="G75" s="47"/>
       <c r="H75" s="6" t="s">
         <v>28</v>
       </c>
@@ -4377,30 +4383,30 @@
       <c r="J75" s="6"/>
       <c r="K75" s="6"/>
       <c r="L75" s="39"/>
-      <c r="M75" s="40"/>
-      <c r="N75" s="40"/>
-      <c r="O75" s="40"/>
+      <c r="M75" s="41"/>
+      <c r="N75" s="41"/>
+      <c r="O75" s="41"/>
       <c r="P75" s="39"/>
       <c r="Q75" s="39"/>
       <c r="R75" s="39"/>
     </row>
     <row r="76" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="41" t="s">
+      <c r="B76" s="46" t="s">
         <v>244</v>
       </c>
-      <c r="C76" s="41" t="s">
+      <c r="C76" s="46" t="s">
         <v>245</v>
       </c>
-      <c r="D76" s="42" t="s">
+      <c r="D76" s="50" t="s">
         <v>150</v>
       </c>
-      <c r="E76" s="45" t="s">
+      <c r="E76" s="52" t="s">
         <v>252</v>
       </c>
-      <c r="F76" s="44" t="s">
+      <c r="F76" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="G76" s="43" t="s">
+      <c r="G76" s="47" t="s">
         <v>118</v>
       </c>
       <c r="H76" s="6" t="s">
@@ -4414,13 +4420,13 @@
       <c r="L76" s="39">
         <v>53273.100258999999</v>
       </c>
-      <c r="M76" s="40">
+      <c r="M76" s="41">
         <v>35.131802046373203</v>
       </c>
-      <c r="N76" s="40">
+      <c r="N76" s="41">
         <v>34.894240188598602</v>
       </c>
-      <c r="O76" s="40">
+      <c r="O76" s="41">
         <v>35.321784973144503</v>
       </c>
       <c r="P76" s="39">
@@ -4434,12 +4440,12 @@
       </c>
     </row>
     <row r="77" spans="2:18" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="41"/>
-      <c r="C77" s="41"/>
-      <c r="D77" s="42"/>
-      <c r="E77" s="45"/>
-      <c r="F77" s="44"/>
-      <c r="G77" s="43"/>
+      <c r="B77" s="46"/>
+      <c r="C77" s="46"/>
+      <c r="D77" s="50"/>
+      <c r="E77" s="52"/>
+      <c r="F77" s="48"/>
+      <c r="G77" s="47"/>
       <c r="H77" s="6" t="s">
         <v>92</v>
       </c>
@@ -4449,9 +4455,9 @@
       <c r="J77" s="6"/>
       <c r="K77" s="6"/>
       <c r="L77" s="39"/>
-      <c r="M77" s="40"/>
-      <c r="N77" s="40"/>
-      <c r="O77" s="40"/>
+      <c r="M77" s="41"/>
+      <c r="N77" s="41"/>
+      <c r="O77" s="41"/>
       <c r="P77" s="39"/>
       <c r="Q77" s="39"/>
       <c r="R77" s="39"/>
@@ -4553,22 +4559,22 @@
       </c>
     </row>
     <row r="80" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B80" s="41" t="s">
+      <c r="B80" s="46" t="s">
         <v>125</v>
       </c>
-      <c r="C80" s="41" t="s">
+      <c r="C80" s="46" t="s">
         <v>126</v>
       </c>
-      <c r="D80" s="42" t="s">
+      <c r="D80" s="50" t="s">
         <v>173</v>
       </c>
-      <c r="E80" s="46" t="s">
+      <c r="E80" s="49" t="s">
         <v>242</v>
       </c>
-      <c r="F80" s="44" t="s">
+      <c r="F80" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="G80" s="43" t="s">
+      <c r="G80" s="47" t="s">
         <v>241</v>
       </c>
       <c r="H80" s="6" t="s">
@@ -4582,13 +4588,13 @@
       <c r="L80" s="39">
         <v>5758.6387889999996</v>
       </c>
-      <c r="M80" s="40">
+      <c r="M80" s="41">
         <v>31.7860839974736</v>
       </c>
-      <c r="N80" s="40">
+      <c r="N80" s="41">
         <v>30.4293422698975</v>
       </c>
-      <c r="O80" s="40">
+      <c r="O80" s="41">
         <v>33.222751617431598</v>
       </c>
       <c r="P80" s="39">
@@ -4602,12 +4608,12 @@
       </c>
     </row>
     <row r="81" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B81" s="41"/>
-      <c r="C81" s="41"/>
-      <c r="D81" s="42"/>
-      <c r="E81" s="46"/>
-      <c r="F81" s="44"/>
-      <c r="G81" s="43"/>
+      <c r="B81" s="46"/>
+      <c r="C81" s="46"/>
+      <c r="D81" s="50"/>
+      <c r="E81" s="49"/>
+      <c r="F81" s="48"/>
+      <c r="G81" s="47"/>
       <c r="H81" s="6" t="s">
         <v>202</v>
       </c>
@@ -4617,31 +4623,31 @@
       <c r="J81" s="6"/>
       <c r="K81" s="6"/>
       <c r="L81" s="39"/>
-      <c r="M81" s="40"/>
-      <c r="N81" s="40"/>
-      <c r="O81" s="40"/>
+      <c r="M81" s="41"/>
+      <c r="N81" s="41"/>
+      <c r="O81" s="41"/>
       <c r="P81" s="39"/>
       <c r="Q81" s="39"/>
       <c r="R81" s="39"/>
     </row>
     <row r="82" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="33"/>
-      <c r="B82" s="41" t="s">
+      <c r="B82" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="C82" s="41" t="s">
+      <c r="C82" s="46" t="s">
         <v>127</v>
       </c>
-      <c r="D82" s="42" t="s">
+      <c r="D82" s="50" t="s">
         <v>179</v>
       </c>
-      <c r="E82" s="46" t="s">
+      <c r="E82" s="49" t="s">
         <v>253</v>
       </c>
-      <c r="F82" s="44" t="s">
+      <c r="F82" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="G82" s="43"/>
+      <c r="G82" s="47"/>
       <c r="H82" s="6" t="s">
         <v>107</v>
       </c>
@@ -4651,13 +4657,13 @@
       <c r="L82" s="39">
         <v>61758.378693999999</v>
       </c>
-      <c r="M82" s="40">
+      <c r="M82" s="41">
         <v>34.328852775604901</v>
       </c>
-      <c r="N82" s="40">
+      <c r="N82" s="41">
         <v>33.196968078613303</v>
       </c>
-      <c r="O82" s="40">
+      <c r="O82" s="41">
         <v>34.815696716308601</v>
       </c>
       <c r="P82" s="39">
@@ -4672,12 +4678,12 @@
     </row>
     <row r="83" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A83" s="33"/>
-      <c r="B83" s="44"/>
-      <c r="C83" s="44"/>
-      <c r="D83" s="43"/>
-      <c r="E83" s="46"/>
-      <c r="F83" s="44"/>
-      <c r="G83" s="44"/>
+      <c r="B83" s="48"/>
+      <c r="C83" s="48"/>
+      <c r="D83" s="47"/>
+      <c r="E83" s="49"/>
+      <c r="F83" s="48"/>
+      <c r="G83" s="48"/>
       <c r="H83" s="8" t="s">
         <v>128</v>
       </c>
@@ -4690,22 +4696,22 @@
       <c r="K83" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="L83" s="48"/>
-      <c r="M83" s="49"/>
-      <c r="N83" s="49"/>
-      <c r="O83" s="49"/>
-      <c r="P83" s="48"/>
-      <c r="Q83" s="48"/>
-      <c r="R83" s="48"/>
+      <c r="L83" s="40"/>
+      <c r="M83" s="42"/>
+      <c r="N83" s="42"/>
+      <c r="O83" s="42"/>
+      <c r="P83" s="40"/>
+      <c r="Q83" s="40"/>
+      <c r="R83" s="40"/>
     </row>
     <row r="84" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A84" s="33"/>
-      <c r="B84" s="44"/>
-      <c r="C84" s="44"/>
-      <c r="D84" s="43"/>
-      <c r="E84" s="46"/>
-      <c r="F84" s="44"/>
-      <c r="G84" s="44"/>
+      <c r="B84" s="48"/>
+      <c r="C84" s="48"/>
+      <c r="D84" s="47"/>
+      <c r="E84" s="49"/>
+      <c r="F84" s="48"/>
+      <c r="G84" s="48"/>
       <c r="H84" s="8" t="s">
         <v>80</v>
       </c>
@@ -4718,22 +4724,22 @@
       <c r="K84" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="L84" s="48"/>
-      <c r="M84" s="49"/>
-      <c r="N84" s="49"/>
-      <c r="O84" s="49"/>
-      <c r="P84" s="48"/>
-      <c r="Q84" s="48"/>
-      <c r="R84" s="48"/>
+      <c r="L84" s="40"/>
+      <c r="M84" s="42"/>
+      <c r="N84" s="42"/>
+      <c r="O84" s="42"/>
+      <c r="P84" s="40"/>
+      <c r="Q84" s="40"/>
+      <c r="R84" s="40"/>
     </row>
     <row r="85" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A85" s="33"/>
-      <c r="B85" s="44"/>
-      <c r="C85" s="44"/>
-      <c r="D85" s="43"/>
-      <c r="E85" s="46"/>
-      <c r="F85" s="44"/>
-      <c r="G85" s="44"/>
+      <c r="B85" s="48"/>
+      <c r="C85" s="48"/>
+      <c r="D85" s="47"/>
+      <c r="E85" s="49"/>
+      <c r="F85" s="48"/>
+      <c r="G85" s="48"/>
       <c r="H85" s="8" t="s">
         <v>65</v>
       </c>
@@ -4742,22 +4748,22 @@
       </c>
       <c r="J85" s="6"/>
       <c r="K85" s="6"/>
-      <c r="L85" s="48"/>
-      <c r="M85" s="49"/>
-      <c r="N85" s="49"/>
-      <c r="O85" s="49"/>
-      <c r="P85" s="48"/>
-      <c r="Q85" s="48"/>
-      <c r="R85" s="48"/>
+      <c r="L85" s="40"/>
+      <c r="M85" s="42"/>
+      <c r="N85" s="42"/>
+      <c r="O85" s="42"/>
+      <c r="P85" s="40"/>
+      <c r="Q85" s="40"/>
+      <c r="R85" s="40"/>
     </row>
     <row r="86" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A86" s="33"/>
-      <c r="B86" s="44"/>
-      <c r="C86" s="44"/>
-      <c r="D86" s="43"/>
-      <c r="E86" s="46"/>
-      <c r="F86" s="44"/>
-      <c r="G86" s="44"/>
+      <c r="B86" s="48"/>
+      <c r="C86" s="48"/>
+      <c r="D86" s="47"/>
+      <c r="E86" s="49"/>
+      <c r="F86" s="48"/>
+      <c r="G86" s="48"/>
       <c r="H86" s="8" t="s">
         <v>201</v>
       </c>
@@ -4766,13 +4772,13 @@
       </c>
       <c r="J86" s="6"/>
       <c r="K86" s="6"/>
-      <c r="L86" s="48"/>
-      <c r="M86" s="49"/>
-      <c r="N86" s="49"/>
-      <c r="O86" s="49"/>
-      <c r="P86" s="48"/>
-      <c r="Q86" s="48"/>
-      <c r="R86" s="48"/>
+      <c r="L86" s="40"/>
+      <c r="M86" s="42"/>
+      <c r="N86" s="42"/>
+      <c r="O86" s="42"/>
+      <c r="P86" s="40"/>
+      <c r="Q86" s="40"/>
+      <c r="R86" s="40"/>
     </row>
     <row r="87" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A87" s="33"/>
@@ -5608,6 +5614,268 @@
   </sheetData>
   <autoFilter ref="B1:K1" xr:uid="{18583828-6250-4FDF-9DB5-A7ECC517AA61}"/>
   <mergeCells count="286">
+    <mergeCell ref="L80:L81"/>
+    <mergeCell ref="M80:M81"/>
+    <mergeCell ref="N80:N81"/>
+    <mergeCell ref="O80:O81"/>
+    <mergeCell ref="P80:P81"/>
+    <mergeCell ref="Q80:Q81"/>
+    <mergeCell ref="R80:R81"/>
+    <mergeCell ref="L74:L75"/>
+    <mergeCell ref="M74:M75"/>
+    <mergeCell ref="N74:N75"/>
+    <mergeCell ref="O74:O75"/>
+    <mergeCell ref="P74:P75"/>
+    <mergeCell ref="Q74:Q75"/>
+    <mergeCell ref="R74:R75"/>
+    <mergeCell ref="L76:L77"/>
+    <mergeCell ref="M76:M77"/>
+    <mergeCell ref="N76:N77"/>
+    <mergeCell ref="O76:O77"/>
+    <mergeCell ref="P76:P77"/>
+    <mergeCell ref="Q76:Q77"/>
+    <mergeCell ref="R76:R77"/>
+    <mergeCell ref="N53:N56"/>
+    <mergeCell ref="O53:O56"/>
+    <mergeCell ref="P53:P56"/>
+    <mergeCell ref="Q53:Q56"/>
+    <mergeCell ref="R53:R56"/>
+    <mergeCell ref="L61:L62"/>
+    <mergeCell ref="M61:M62"/>
+    <mergeCell ref="N61:N62"/>
+    <mergeCell ref="O61:O62"/>
+    <mergeCell ref="P61:P62"/>
+    <mergeCell ref="Q61:Q62"/>
+    <mergeCell ref="R61:R62"/>
+    <mergeCell ref="N44:N46"/>
+    <mergeCell ref="O44:O46"/>
+    <mergeCell ref="P44:P46"/>
+    <mergeCell ref="Q44:Q46"/>
+    <mergeCell ref="R44:R46"/>
+    <mergeCell ref="L40:L41"/>
+    <mergeCell ref="M40:M41"/>
+    <mergeCell ref="N40:N41"/>
+    <mergeCell ref="O40:O41"/>
+    <mergeCell ref="P40:P41"/>
+    <mergeCell ref="Q40:Q41"/>
+    <mergeCell ref="R40:R41"/>
+    <mergeCell ref="R17:R18"/>
+    <mergeCell ref="Q10:Q12"/>
+    <mergeCell ref="R10:R12"/>
+    <mergeCell ref="N13:N16"/>
+    <mergeCell ref="O13:O16"/>
+    <mergeCell ref="N38:N39"/>
+    <mergeCell ref="O38:O39"/>
+    <mergeCell ref="P38:P39"/>
+    <mergeCell ref="Q38:Q39"/>
+    <mergeCell ref="R38:R39"/>
+    <mergeCell ref="N31:N34"/>
+    <mergeCell ref="O31:O34"/>
+    <mergeCell ref="P31:P34"/>
+    <mergeCell ref="Q31:Q34"/>
+    <mergeCell ref="R31:R34"/>
+    <mergeCell ref="N35:N37"/>
+    <mergeCell ref="O35:O37"/>
+    <mergeCell ref="P35:P37"/>
+    <mergeCell ref="Q35:Q37"/>
+    <mergeCell ref="R35:R37"/>
+    <mergeCell ref="R19:R20"/>
+    <mergeCell ref="N17:N18"/>
+    <mergeCell ref="O17:O18"/>
+    <mergeCell ref="P17:P18"/>
+    <mergeCell ref="L24:L25"/>
+    <mergeCell ref="M24:M25"/>
+    <mergeCell ref="N24:N25"/>
+    <mergeCell ref="O24:O25"/>
+    <mergeCell ref="P24:P25"/>
+    <mergeCell ref="Q24:Q25"/>
+    <mergeCell ref="R24:R25"/>
+    <mergeCell ref="L19:L20"/>
+    <mergeCell ref="M19:M20"/>
+    <mergeCell ref="N19:N20"/>
+    <mergeCell ref="O19:O20"/>
+    <mergeCell ref="P19:P20"/>
+    <mergeCell ref="Q19:Q20"/>
+    <mergeCell ref="L38:L39"/>
+    <mergeCell ref="M38:M39"/>
+    <mergeCell ref="L44:L46"/>
+    <mergeCell ref="M44:M46"/>
+    <mergeCell ref="M53:M56"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="C4:C7"/>
+    <mergeCell ref="D4:D7"/>
+    <mergeCell ref="E4:E7"/>
+    <mergeCell ref="F4:F7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="L10:L12"/>
+    <mergeCell ref="M10:M12"/>
+    <mergeCell ref="L31:L34"/>
+    <mergeCell ref="M31:M34"/>
+    <mergeCell ref="L35:L37"/>
+    <mergeCell ref="M35:M37"/>
+    <mergeCell ref="M17:M18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="L17:L18"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="N63:N69"/>
+    <mergeCell ref="O63:O69"/>
+    <mergeCell ref="P63:P69"/>
+    <mergeCell ref="Q63:Q69"/>
+    <mergeCell ref="R63:R69"/>
+    <mergeCell ref="L71:L72"/>
+    <mergeCell ref="M71:M72"/>
+    <mergeCell ref="N71:N72"/>
+    <mergeCell ref="B76:B77"/>
+    <mergeCell ref="C76:C77"/>
+    <mergeCell ref="D76:D77"/>
+    <mergeCell ref="E76:E77"/>
+    <mergeCell ref="O71:O72"/>
+    <mergeCell ref="P71:P72"/>
+    <mergeCell ref="Q71:Q72"/>
+    <mergeCell ref="R71:R72"/>
+    <mergeCell ref="F76:F77"/>
+    <mergeCell ref="G76:G77"/>
+    <mergeCell ref="G63:G69"/>
+    <mergeCell ref="B63:B69"/>
+    <mergeCell ref="C63:C69"/>
+    <mergeCell ref="D63:D69"/>
+    <mergeCell ref="E63:E69"/>
+    <mergeCell ref="F63:F69"/>
+    <mergeCell ref="Q17:Q18"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="N4:N7"/>
+    <mergeCell ref="O4:O7"/>
+    <mergeCell ref="P4:P7"/>
+    <mergeCell ref="Q4:Q7"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="O8:O9"/>
+    <mergeCell ref="P8:P9"/>
+    <mergeCell ref="Q8:Q9"/>
+    <mergeCell ref="L4:L7"/>
+    <mergeCell ref="M4:M7"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="M8:M9"/>
+    <mergeCell ref="L13:L16"/>
+    <mergeCell ref="M13:M16"/>
+    <mergeCell ref="N10:N12"/>
+    <mergeCell ref="O10:O12"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="E10:E12"/>
+    <mergeCell ref="D13:D16"/>
+    <mergeCell ref="E13:E16"/>
+    <mergeCell ref="R4:R7"/>
+    <mergeCell ref="R8:R9"/>
+    <mergeCell ref="G4:G7"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="F10:F12"/>
+    <mergeCell ref="F13:F16"/>
+    <mergeCell ref="G13:G16"/>
+    <mergeCell ref="G10:G12"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="P10:P12"/>
+    <mergeCell ref="P13:P16"/>
+    <mergeCell ref="Q13:Q16"/>
+    <mergeCell ref="R13:R16"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="D35:D37"/>
+    <mergeCell ref="E35:E37"/>
+    <mergeCell ref="F35:F37"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="C31:C34"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D31:D34"/>
+    <mergeCell ref="E31:E34"/>
+    <mergeCell ref="F31:F34"/>
+    <mergeCell ref="G31:G34"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="C13:C16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="G38:G39"/>
+    <mergeCell ref="G35:G37"/>
+    <mergeCell ref="F44:F46"/>
+    <mergeCell ref="G44:G46"/>
+    <mergeCell ref="G40:G41"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="D44:D46"/>
+    <mergeCell ref="E44:E46"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="E40:E41"/>
+    <mergeCell ref="F40:F41"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="B53:B56"/>
+    <mergeCell ref="C53:C56"/>
+    <mergeCell ref="D53:D56"/>
+    <mergeCell ref="E53:E56"/>
+    <mergeCell ref="F53:F56"/>
+    <mergeCell ref="G53:G56"/>
+    <mergeCell ref="B50:B52"/>
+    <mergeCell ref="D50:D52"/>
+    <mergeCell ref="E50:E52"/>
+    <mergeCell ref="F50:F52"/>
+    <mergeCell ref="G50:G52"/>
+    <mergeCell ref="C50:C52"/>
+    <mergeCell ref="G48:G49"/>
+    <mergeCell ref="F48:F49"/>
+    <mergeCell ref="E48:E49"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="G74:G75"/>
+    <mergeCell ref="F74:F75"/>
+    <mergeCell ref="D74:D75"/>
+    <mergeCell ref="B74:B75"/>
+    <mergeCell ref="C74:C75"/>
+    <mergeCell ref="E74:E75"/>
+    <mergeCell ref="F61:F62"/>
+    <mergeCell ref="G61:G62"/>
+    <mergeCell ref="G71:G72"/>
+    <mergeCell ref="F71:F72"/>
+    <mergeCell ref="E71:E72"/>
+    <mergeCell ref="B61:B62"/>
+    <mergeCell ref="C61:C62"/>
+    <mergeCell ref="D61:D62"/>
+    <mergeCell ref="E61:E62"/>
+    <mergeCell ref="D71:D72"/>
+    <mergeCell ref="C71:C72"/>
+    <mergeCell ref="B71:B72"/>
+    <mergeCell ref="C80:C81"/>
+    <mergeCell ref="B80:B81"/>
+    <mergeCell ref="G82:G86"/>
+    <mergeCell ref="G80:G81"/>
+    <mergeCell ref="F80:F81"/>
+    <mergeCell ref="E80:E81"/>
+    <mergeCell ref="D80:D81"/>
+    <mergeCell ref="B82:B86"/>
+    <mergeCell ref="C82:C86"/>
+    <mergeCell ref="D82:D86"/>
+    <mergeCell ref="E82:E86"/>
+    <mergeCell ref="F82:F86"/>
     <mergeCell ref="L82:L86"/>
     <mergeCell ref="M82:M86"/>
     <mergeCell ref="N82:N86"/>
@@ -5632,268 +5900,6 @@
     <mergeCell ref="L53:L56"/>
     <mergeCell ref="L63:L69"/>
     <mergeCell ref="M63:M69"/>
-    <mergeCell ref="C80:C81"/>
-    <mergeCell ref="B80:B81"/>
-    <mergeCell ref="G82:G86"/>
-    <mergeCell ref="G80:G81"/>
-    <mergeCell ref="F80:F81"/>
-    <mergeCell ref="E80:E81"/>
-    <mergeCell ref="D80:D81"/>
-    <mergeCell ref="B82:B86"/>
-    <mergeCell ref="C82:C86"/>
-    <mergeCell ref="D82:D86"/>
-    <mergeCell ref="E82:E86"/>
-    <mergeCell ref="F82:F86"/>
-    <mergeCell ref="G74:G75"/>
-    <mergeCell ref="F74:F75"/>
-    <mergeCell ref="D74:D75"/>
-    <mergeCell ref="B74:B75"/>
-    <mergeCell ref="C74:C75"/>
-    <mergeCell ref="E74:E75"/>
-    <mergeCell ref="F61:F62"/>
-    <mergeCell ref="G61:G62"/>
-    <mergeCell ref="G71:G72"/>
-    <mergeCell ref="F71:F72"/>
-    <mergeCell ref="E71:E72"/>
-    <mergeCell ref="B61:B62"/>
-    <mergeCell ref="C61:C62"/>
-    <mergeCell ref="D61:D62"/>
-    <mergeCell ref="E61:E62"/>
-    <mergeCell ref="D71:D72"/>
-    <mergeCell ref="C71:C72"/>
-    <mergeCell ref="B71:B72"/>
-    <mergeCell ref="F40:F41"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="B53:B56"/>
-    <mergeCell ref="C53:C56"/>
-    <mergeCell ref="D53:D56"/>
-    <mergeCell ref="E53:E56"/>
-    <mergeCell ref="F53:F56"/>
-    <mergeCell ref="G53:G56"/>
-    <mergeCell ref="B50:B52"/>
-    <mergeCell ref="D50:D52"/>
-    <mergeCell ref="E50:E52"/>
-    <mergeCell ref="F50:F52"/>
-    <mergeCell ref="G50:G52"/>
-    <mergeCell ref="C50:C52"/>
-    <mergeCell ref="G48:G49"/>
-    <mergeCell ref="F48:F49"/>
-    <mergeCell ref="E48:E49"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="C13:C16"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="G38:G39"/>
-    <mergeCell ref="G35:G37"/>
-    <mergeCell ref="F44:F46"/>
-    <mergeCell ref="G44:G46"/>
-    <mergeCell ref="G40:G41"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="F38:F39"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="D44:D46"/>
-    <mergeCell ref="E44:E46"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="E40:E41"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="D35:D37"/>
-    <mergeCell ref="E35:E37"/>
-    <mergeCell ref="F35:F37"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="B31:B34"/>
-    <mergeCell ref="C31:C34"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D31:D34"/>
-    <mergeCell ref="E31:E34"/>
-    <mergeCell ref="F31:F34"/>
-    <mergeCell ref="G31:G34"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="R4:R7"/>
-    <mergeCell ref="R8:R9"/>
-    <mergeCell ref="G4:G7"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="F10:F12"/>
-    <mergeCell ref="F13:F16"/>
-    <mergeCell ref="G13:G16"/>
-    <mergeCell ref="G10:G12"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="P10:P12"/>
-    <mergeCell ref="P13:P16"/>
-    <mergeCell ref="Q13:Q16"/>
-    <mergeCell ref="R13:R16"/>
-    <mergeCell ref="Q17:Q18"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="N4:N7"/>
-    <mergeCell ref="O4:O7"/>
-    <mergeCell ref="P4:P7"/>
-    <mergeCell ref="Q4:Q7"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="O8:O9"/>
-    <mergeCell ref="P8:P9"/>
-    <mergeCell ref="Q8:Q9"/>
-    <mergeCell ref="L4:L7"/>
-    <mergeCell ref="M4:M7"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="M8:M9"/>
-    <mergeCell ref="L13:L16"/>
-    <mergeCell ref="M13:M16"/>
-    <mergeCell ref="N10:N12"/>
-    <mergeCell ref="O10:O12"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="E10:E12"/>
-    <mergeCell ref="D13:D16"/>
-    <mergeCell ref="E13:E16"/>
-    <mergeCell ref="N63:N69"/>
-    <mergeCell ref="O63:O69"/>
-    <mergeCell ref="P63:P69"/>
-    <mergeCell ref="Q63:Q69"/>
-    <mergeCell ref="R63:R69"/>
-    <mergeCell ref="L71:L72"/>
-    <mergeCell ref="M71:M72"/>
-    <mergeCell ref="N71:N72"/>
-    <mergeCell ref="B76:B77"/>
-    <mergeCell ref="C76:C77"/>
-    <mergeCell ref="D76:D77"/>
-    <mergeCell ref="E76:E77"/>
-    <mergeCell ref="O71:O72"/>
-    <mergeCell ref="P71:P72"/>
-    <mergeCell ref="Q71:Q72"/>
-    <mergeCell ref="R71:R72"/>
-    <mergeCell ref="F76:F77"/>
-    <mergeCell ref="G76:G77"/>
-    <mergeCell ref="G63:G69"/>
-    <mergeCell ref="B63:B69"/>
-    <mergeCell ref="C63:C69"/>
-    <mergeCell ref="D63:D69"/>
-    <mergeCell ref="E63:E69"/>
-    <mergeCell ref="F63:F69"/>
-    <mergeCell ref="L38:L39"/>
-    <mergeCell ref="M38:M39"/>
-    <mergeCell ref="L44:L46"/>
-    <mergeCell ref="M44:M46"/>
-    <mergeCell ref="M53:M56"/>
-    <mergeCell ref="B4:B7"/>
-    <mergeCell ref="C4:C7"/>
-    <mergeCell ref="D4:D7"/>
-    <mergeCell ref="E4:E7"/>
-    <mergeCell ref="F4:F7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="L10:L12"/>
-    <mergeCell ref="M10:M12"/>
-    <mergeCell ref="L31:L34"/>
-    <mergeCell ref="M31:M34"/>
-    <mergeCell ref="L35:L37"/>
-    <mergeCell ref="M35:M37"/>
-    <mergeCell ref="M17:M18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="L17:L18"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="L24:L25"/>
-    <mergeCell ref="M24:M25"/>
-    <mergeCell ref="N24:N25"/>
-    <mergeCell ref="O24:O25"/>
-    <mergeCell ref="P24:P25"/>
-    <mergeCell ref="Q24:Q25"/>
-    <mergeCell ref="R24:R25"/>
-    <mergeCell ref="L19:L20"/>
-    <mergeCell ref="M19:M20"/>
-    <mergeCell ref="N19:N20"/>
-    <mergeCell ref="O19:O20"/>
-    <mergeCell ref="P19:P20"/>
-    <mergeCell ref="Q19:Q20"/>
-    <mergeCell ref="R17:R18"/>
-    <mergeCell ref="Q10:Q12"/>
-    <mergeCell ref="R10:R12"/>
-    <mergeCell ref="N13:N16"/>
-    <mergeCell ref="O13:O16"/>
-    <mergeCell ref="N38:N39"/>
-    <mergeCell ref="O38:O39"/>
-    <mergeCell ref="P38:P39"/>
-    <mergeCell ref="Q38:Q39"/>
-    <mergeCell ref="R38:R39"/>
-    <mergeCell ref="N31:N34"/>
-    <mergeCell ref="O31:O34"/>
-    <mergeCell ref="P31:P34"/>
-    <mergeCell ref="Q31:Q34"/>
-    <mergeCell ref="R31:R34"/>
-    <mergeCell ref="N35:N37"/>
-    <mergeCell ref="O35:O37"/>
-    <mergeCell ref="P35:P37"/>
-    <mergeCell ref="Q35:Q37"/>
-    <mergeCell ref="R35:R37"/>
-    <mergeCell ref="R19:R20"/>
-    <mergeCell ref="N17:N18"/>
-    <mergeCell ref="O17:O18"/>
-    <mergeCell ref="P17:P18"/>
-    <mergeCell ref="N44:N46"/>
-    <mergeCell ref="O44:O46"/>
-    <mergeCell ref="P44:P46"/>
-    <mergeCell ref="Q44:Q46"/>
-    <mergeCell ref="R44:R46"/>
-    <mergeCell ref="L40:L41"/>
-    <mergeCell ref="M40:M41"/>
-    <mergeCell ref="N40:N41"/>
-    <mergeCell ref="O40:O41"/>
-    <mergeCell ref="P40:P41"/>
-    <mergeCell ref="Q40:Q41"/>
-    <mergeCell ref="R40:R41"/>
-    <mergeCell ref="N53:N56"/>
-    <mergeCell ref="O53:O56"/>
-    <mergeCell ref="P53:P56"/>
-    <mergeCell ref="Q53:Q56"/>
-    <mergeCell ref="R53:R56"/>
-    <mergeCell ref="L61:L62"/>
-    <mergeCell ref="M61:M62"/>
-    <mergeCell ref="N61:N62"/>
-    <mergeCell ref="O61:O62"/>
-    <mergeCell ref="P61:P62"/>
-    <mergeCell ref="Q61:Q62"/>
-    <mergeCell ref="R61:R62"/>
-    <mergeCell ref="L80:L81"/>
-    <mergeCell ref="M80:M81"/>
-    <mergeCell ref="N80:N81"/>
-    <mergeCell ref="O80:O81"/>
-    <mergeCell ref="P80:P81"/>
-    <mergeCell ref="Q80:Q81"/>
-    <mergeCell ref="R80:R81"/>
-    <mergeCell ref="L74:L75"/>
-    <mergeCell ref="M74:M75"/>
-    <mergeCell ref="N74:N75"/>
-    <mergeCell ref="O74:O75"/>
-    <mergeCell ref="P74:P75"/>
-    <mergeCell ref="Q74:Q75"/>
-    <mergeCell ref="R74:R75"/>
-    <mergeCell ref="L76:L77"/>
-    <mergeCell ref="M76:M77"/>
-    <mergeCell ref="N76:N77"/>
-    <mergeCell ref="O76:O77"/>
-    <mergeCell ref="P76:P77"/>
-    <mergeCell ref="Q76:Q77"/>
-    <mergeCell ref="R76:R77"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5904,7 +5910,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AFAD807-1D69-42B0-8283-E5A2E6237B5C}">
   <dimension ref="A1:V91"/>
   <sheetViews>
-    <sheetView topLeftCell="B13" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -6083,6 +6089,14 @@
         <v>342</v>
       </c>
     </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>345</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>346</v>
+      </c>
+    </row>
     <row r="78" spans="17:22" x14ac:dyDescent="0.25">
       <c r="Q78" s="15"/>
       <c r="U78" s="15"/>

</xml_diff>